<commit_message>
Johns Commit 2: control table and vin upload changes. SS test edits. will verify details on policy summary page after endorsement as well as in the generated renewal image.
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VinUploadOnCurrentTerm_AZ_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VinUploadOnCurrentTerm_AZ_SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gw3eraj\Documents\Project\Sprint work\Sprint 32\User Stories\PAS-14532\Upload files PAS-14532\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="88">
   <si>
     <t>VIN</t>
   </si>
@@ -134,9 +134,6 @@
     <t>RESTRAINTS_DISCOUNT</t>
   </si>
   <si>
-    <t>SYMBOL_2000</t>
-  </si>
-  <si>
     <t>2WD</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>KIA</t>
   </si>
   <si>
-    <t>SOUL +/!/SPORT</t>
-  </si>
-  <si>
     <t>4D WAG</t>
   </si>
   <si>
@@ -185,9 +179,6 @@
     <t>2.0L L4</t>
   </si>
   <si>
-    <t>SOUL</t>
-  </si>
-  <si>
     <t>JT2AE91A&amp;M</t>
   </si>
   <si>
@@ -209,12 +200,6 @@
     <t>NONE</t>
   </si>
   <si>
-    <t>TOYOTA</t>
-  </si>
-  <si>
-    <t>COROLLA</t>
-  </si>
-  <si>
     <t>0007</t>
   </si>
   <si>
@@ -240,6 +225,69 @@
   </si>
   <si>
     <t>SYMBOL_2018</t>
+  </si>
+  <si>
+    <t>1FTRE142&amp;Y</t>
+  </si>
+  <si>
+    <t>FORD</t>
+  </si>
+  <si>
+    <t>ECONOLINE VAN</t>
+  </si>
+  <si>
+    <t>ECONOLINE E150</t>
+  </si>
+  <si>
+    <t>VAN</t>
+  </si>
+  <si>
+    <t>CARGO VAN</t>
+  </si>
+  <si>
+    <t>4.2L V6</t>
+  </si>
+  <si>
+    <t>000E</t>
+  </si>
+  <si>
+    <t>FRONT AIRBAGS</t>
+  </si>
+  <si>
+    <t>N-NONE</t>
+  </si>
+  <si>
+    <t>5NPEU46C&amp;9</t>
+  </si>
+  <si>
+    <t>HYUN</t>
+  </si>
+  <si>
+    <t>SONATA</t>
+  </si>
+  <si>
+    <t>SONATA SE/LIMITED</t>
+  </si>
+  <si>
+    <t>2.4L L4</t>
+  </si>
+  <si>
+    <t>000V</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>B-IMMOBILIZER/KEYLSS ENTRY/ALARM</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>FORD MOTOR</t>
+  </si>
+  <si>
+    <t>HYUNDAI MOTOR</t>
   </si>
 </sst>
 </file>
@@ -301,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -310,6 +358,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -596,21 +650,24 @@
   <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,411 +777,412 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="C2" s="3">
         <v>2010</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="J2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="O2" s="3">
         <v>4</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S2" s="3">
         <v>2</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="U2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V2" s="3">
         <v>2</v>
       </c>
       <c r="W2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X2" s="3">
         <v>2</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Z2" s="3">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="AA2" s="3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="AB2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>20180608</v>
+      </c>
+      <c r="AH2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AD2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG2" s="4">
-        <v>20000101</v>
-      </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1991</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AI2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2010</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="J3" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O3" s="3">
         <v>4</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S3" s="3">
         <v>2</v>
       </c>
-      <c r="T3" s="5" t="s">
-        <v>63</v>
+      <c r="T3" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="U3" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="V3" s="3">
-        <v>2</v>
-      </c>
-      <c r="W3" t="s">
-        <v>38</v>
-      </c>
-      <c r="X3" s="3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="Z3" s="3">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="AA3" s="3">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="AB3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="AD3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AG3" s="4">
         <v>20180608</v>
       </c>
       <c r="AH3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ3" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2000</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="O4" s="6">
+        <v>6</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="6">
+        <v>2</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="V4" s="6">
+        <v>2</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>14</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>24</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>20180608</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AI3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="J5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" s="6">
+        <v>4</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="3">
-        <v>1991</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="S5" s="6">
+        <v>2</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" s="6">
+        <v>2</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>15</v>
+      </c>
+      <c r="AA5" s="6">
         <v>55</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="3">
-        <v>4</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S4" s="3">
-        <v>2</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="U4" t="s">
-        <v>58</v>
-      </c>
-      <c r="V4" s="3">
-        <v>1</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z4" s="3">
-        <v>51</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>50</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG4" s="4">
-        <v>20000101</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ4" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1991</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="O5" s="3">
-        <v>4</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" s="3">
-        <v>2</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="U5" t="s">
-        <v>58</v>
-      </c>
-      <c r="V5" s="3">
-        <v>1</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z5" s="3">
-        <v>51</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>50</v>
-      </c>
       <c r="AB5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="AC5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF5" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="AG5" s="4">
         <v>20180608</v>
       </c>
       <c r="AH5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AI5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>